<commit_message>
added comment citing page
</commit_message>
<xml_diff>
--- a/output/goog-10-k-2024_extracted.xlsx
+++ b/output/goog-10-k-2024_extracted.xlsx
@@ -7,7 +7,8 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="INCOME" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="CASH_FLOWS" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -136,6 +137,36 @@
 </styleSheet>
 </file>
 
+<file path=xl/comments/comment1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>PDF Processor</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0">
+      <text>
+        <t>From page 54 of goog-10-k-2024.pdf</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments/comment2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>PDF Processor</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0">
+      <text>
+        <t>From page 44 of goog-10-k-2024.pdf</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -743,5 +774,134 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Value_1</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Value_2</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Value_3</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Value_4</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Class A share repurchases</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>78</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>9316</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>73</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>11855</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Class C share repurchases</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>450</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>52868</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>306</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>50192</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Total share repurchases(1)</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>528</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>62184</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>379</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>62047</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
reads 3 statements for 10q now, 10k still a mess
</commit_message>
<xml_diff>
--- a/output/goog-10-k-2024_extracted.xlsx
+++ b/output/goog-10-k-2024_extracted.xlsx
@@ -8,7 +8,8 @@
   </bookViews>
   <sheets>
     <sheet name="INCOME" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="CASH_FLOWS" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="CONSOLIDATED_BALANCE_SHEETS" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="CASH_FLOWS" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -153,6 +154,21 @@
 </file>
 
 <file path=xl/comments/comment2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>PDF Processor</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0">
+      <text>
+        <t>From page 43 of goog-10-k-2024.pdf</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments/comment3.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>PDF Processor</author>
@@ -784,6 +800,138 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:I4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr"/>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>None_1</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>None_2</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>None_3</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>None_4</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>$4.0 billion</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>expiring in</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>April 2025</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>and</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>$6.0 billion</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>expiring in</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>April 2028</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>. The interest rates for all credit facilities are determined based on a formula using</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>certain market rates, as well as our progress toward the achievement of certain</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>sustainability</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>goals</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>have</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>been borrowed under the credit facilities.</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
updated page filter to differentiate between paragraph and table
</commit_message>
<xml_diff>
--- a/output/goog-10-k-2024_extracted.xlsx
+++ b/output/goog-10-k-2024_extracted.xlsx
@@ -161,7 +161,7 @@
   <commentList>
     <comment ref="A1" authorId="0" shapeId="0">
       <text>
-        <t>From page 43 of goog-10-k-2024.pdf</t>
+        <t>From page 53 of goog-10-k-2024.pdf</t>
       </text>
     </comment>
   </commentList>
@@ -176,7 +176,7 @@
   <commentList>
     <comment ref="A1" authorId="0" shapeId="0">
       <text>
-        <t>From page 44 of goog-10-k-2024.pdf</t>
+        <t>From page 57 of goog-10-k-2024.pdf</t>
       </text>
     </comment>
   </commentList>
@@ -800,7 +800,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -809,116 +809,531 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr"/>
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>None_1</t>
+          <t>Year Ended December 31, 2023</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>None_2</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>None_3</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>None_4</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>$4.0 billion</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>expiring in</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>April 2025</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>and</t>
+          <t>Year Ended December 31, 2024</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>$6.0 billion</t>
+          <t>Cash and cash equivalents</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>expiring in</t>
+          <t>24048</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>April 2028</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>. The interest rates for all credit facilities are determined based on a formula using</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr"/>
+          <t>23466</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>certain market rates, as well as our progress toward the achievement of certain</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr"/>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>sustainability</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>goals</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>have</t>
+          <t>Marketable securities</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>86868</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>72191</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>been borrowed under the credit facilities.</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr"/>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
+          <t>Total cash, cash equivalents, and marketable securities</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>110916</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>95657</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Accounts receivable, net</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>47964</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>52340</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Other current assets</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>12650</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>15714</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Total current assets</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>171530</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>163711</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Non-marketable securities</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>31008</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>37982</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Deferred income taxes</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>12169</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>17180</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Property and equipment, net</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>134345</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>171036</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Operating lease assets</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>14091</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>13588</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Goodwill</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>29198</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>31885</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Other non-current assets</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>10051</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>14874</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Total assets</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>402392</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>450256</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Accounts payable</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>7493</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>7987</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Accrued compensation and benefits</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>15140</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>15069</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Accrued expenses and other current liabilities</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>46168</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>51228</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Accrued revenue share</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>8876</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>9802</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Deferred revenue</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>4137</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>5036</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Total current liabilities</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>81814</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>89122</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Long-term debt</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>11870</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>10883</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Income taxes payable, non-current</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>8474</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>8782</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Operating lease liabilities</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>12460</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>11691</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Other long-term liabilities</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>4395</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>4694</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Total liabilities</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>119013</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>125172</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Preferred stock, 0.001 par value per share, 100 shares authorized; no shares issued and outstanding</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Class A, Class B, and Class C stock and additional paid-in capital, 0.001 par value per share: 300,000 shares authorized (Class A 180,000, Class B 60,000, Class C 60,000); 12,460 (Class A 5,899, Class B 870, Class C 5,691) and 12,211 (Class A 5,835, Class B 861, Class C 5,515) shares issued and outstanding</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>76534</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>84800</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Accumulated other comprehensive income (loss)</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>-4402</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>-4800</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Retained earnings</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>211247</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>245084</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Total stockholders’ equity</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>283379</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>325084</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Total liabilities and stockholders’ equity</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>402392</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>450256</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -932,7 +1347,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -948,103 +1363,743 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Value_1</t>
+          <t>Year Ended December 31, 2022</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Value_2</t>
+          <t>Year Ended December 31, 2023</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Value_3</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Value_4</t>
+          <t>Year Ended December 31, 2024</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Class A share repurchases</t>
+          <t>Net income</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>78</t>
+          <t>59972</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>9316</t>
+          <t>73795</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>73</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>11855</t>
+          <t>100118</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Class C share repurchases</t>
+          <t>Depreciation of property and equipment</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>450</t>
+          <t>13475</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>52868</t>
+          <t>11946</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>306</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>50192</t>
+          <t>15311</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Total share repurchases(1)</t>
+          <t>Stock-based compensation expense</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>528</t>
+          <t>19362</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>62184</t>
+          <t>22460</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>379</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>62047</t>
+          <t>22785</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Deferred income taxes</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>-8081</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>-7763</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>-5257</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Loss (gain) on debt and equity securities, net</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>5519</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>823</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>-2671</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>3483</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>4330</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>3419</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Accounts receivable, net</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>-2317</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>-7833</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>-5891</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Income taxes, net</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>584</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>523</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>-2418</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Other assets</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>-5046</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>-2143</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>-1397</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Accounts payable</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>707</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>664</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>359</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Accrued expenses and other liabilities</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>3915</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>3937</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>-1161</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Accrued revenue share</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>-445</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>482</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>1059</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Deferred revenue</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>367</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>525</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>1043</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Net cash provided by operating activities</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>91495</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>101746</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>125299</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Purchases of property and equipment</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>-31485</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>-32251</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>-52535</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Purchases of marketable securities</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>-78874</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>-77858</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>-86679</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Maturities and sales of marketable securities</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>97822</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>86672</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>103428</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Purchases of non-marketable securities</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>-2531</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>-3027</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>-5034</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Maturities and sales of non-marketable securities</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>947</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>882</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Acquisitions, net of cash acquired, and purchases of intangible assets</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>-6969</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>-495</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>-2931</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Other investing activities</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>1589</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>-1051</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>-2667</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Net cash used in investing activities</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>-20298</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>-27063</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>-45536</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Net payments related to stock-based award activities</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>-9300</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>-9837</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>-12190</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Repurchases of stock</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>-59296</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>-61504</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>-62222</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Dividend payments</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>-7363</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Proceeds from issuance of debt, net of costs</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>52872</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>10790</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>13589</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Repayments of debt</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>-54068</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>-11550</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>-12701</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Proceeds from sale of interest in consolidated entities, net</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>1154</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Net cash used in financing activities</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>-69757</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>-72093</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>-79733</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Effect of exchange rate changes on cash and cash equivalents</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>-506</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>-421</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>-612</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Net increase (decrease) in cash and cash equivalents</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>934</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>2169</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>-582</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Cash and cash equivalents at beginning of period</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>20945</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>21879</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>24048</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Cash and cash equivalents at end of period</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>21879</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>24048</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>23466</t>
         </is>
       </c>
     </row>

</xml_diff>